<commit_message>
Game Rank solved - kattis
</commit_message>
<xml_diff>
--- a/R E C 0 r D.xlsx
+++ b/R E C 0 r D.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>10812 Beat the Spread!</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>helpme [2.7]</t>
+  </si>
+  <si>
+    <t>11th</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gamerank [3.6]</t>
   </si>
 </sst>
 </file>
@@ -633,7 +639,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,6 +844,12 @@
       <c r="B18" s="10">
         <v>3</v>
       </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">

</xml_diff>